<commit_message>
Login funktioniert + UnitOfWork injiziert
</commit_message>
<xml_diff>
--- a/01_Planning/ProductBurndown.xlsx
+++ b/01_Planning/ProductBurndown.xlsx
@@ -491,142 +491,142 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="46"/>
                 <c:pt idx="0" formatCode="0.0">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -642,11 +642,11 @@
         </c:dLbls>
         <c:gapWidth val="40"/>
         <c:overlap val="-10"/>
-        <c:axId val="469860400"/>
-        <c:axId val="469854912"/>
+        <c:axId val="459422912"/>
+        <c:axId val="459418992"/>
       </c:barChart>
       <c:dateAx>
-        <c:axId val="469860400"/>
+        <c:axId val="459422912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -685,14 +685,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="469854912"/>
+        <c:crossAx val="459418992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="469854912"/>
+        <c:axId val="459418992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -738,7 +738,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="469860400"/>
+        <c:crossAx val="459422912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="25"/>
@@ -1204,7 +1204,7 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1240,7 +1240,7 @@
     </row>
     <row r="3" spans="1:4" ht="20.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B3" s="3">
         <v>0</v>
@@ -1276,7 +1276,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="O11" sqref="O11"/>
+      <selection pane="bottomRight" activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1361,7 +1361,7 @@
       </c>
       <c r="F3" s="4">
         <f>'Sheet 1 - Initial'!A3+C3</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G3" s="4">
         <f>'Sheet 1 - Initial'!B3</f>
@@ -1377,7 +1377,7 @@
       </c>
       <c r="J3" s="6">
         <f>MAX(IF(OR(ISBLANK(D3),ISBLANK(E3)),F3-'Sheet 1 - Initial'!D3*B3,F3-D3),0)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K3" s="7">
         <f>IF(OR(ISBLANK(D3),ISBLANK(E3)),'Sheet 1 - Initial'!D3,H3/(I3+E3))</f>
@@ -1394,10 +1394,12 @@
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="E4" s="3">
+        <v>7</v>
+      </c>
       <c r="F4" s="4">
         <f t="shared" ref="F4:F48" si="2">J3+C4</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G4" s="4">
         <f t="shared" ref="G4:G48" si="3">H3</f>
@@ -1413,7 +1415,7 @@
       </c>
       <c r="J4" s="4">
         <f t="shared" ref="J4:J48" si="5">MAX(IF(OR(ISBLANK(D4),ISBLANK(E4)),F4-K3*B4,F4-D4),0)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K4" s="7">
         <f t="shared" ref="K4:K48" si="6">IF(OR(ISBLANK(D4),ISBLANK(E4)),K3,H4/(I4+E4))</f>
@@ -1426,14 +1428,16 @@
         <v>41405</v>
       </c>
       <c r="B5" s="3">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+      <c r="E5" s="3">
+        <v>6</v>
+      </c>
       <c r="F5" s="4">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G5" s="4">
         <f t="shared" si="3"/>
@@ -1445,11 +1449,11 @@
       </c>
       <c r="I5" s="4">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="J5" s="4">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K5" s="7">
         <f t="shared" si="6"/>
@@ -1462,14 +1466,14 @@
         <v>41412</v>
       </c>
       <c r="B6" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="4">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G6" s="4">
         <f t="shared" si="3"/>
@@ -1481,11 +1485,11 @@
       </c>
       <c r="I6" s="4">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="J6" s="4">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K6" s="7">
         <f t="shared" si="6"/>
@@ -1505,7 +1509,7 @@
       <c r="E7" s="3"/>
       <c r="F7" s="4">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G7" s="4">
         <f t="shared" si="3"/>
@@ -1517,11 +1521,11 @@
       </c>
       <c r="I7" s="4">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="J7" s="4">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K7" s="7">
         <f t="shared" si="6"/>
@@ -1541,7 +1545,7 @@
       <c r="E8" s="3"/>
       <c r="F8" s="4">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G8" s="4">
         <f t="shared" si="3"/>
@@ -1553,11 +1557,11 @@
       </c>
       <c r="I8" s="4">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="J8" s="4">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K8" s="7">
         <f t="shared" si="6"/>
@@ -1577,7 +1581,7 @@
       <c r="E9" s="3"/>
       <c r="F9" s="4">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G9" s="4">
         <f t="shared" si="3"/>
@@ -1589,11 +1593,11 @@
       </c>
       <c r="I9" s="4">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="J9" s="4">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K9" s="7">
         <f t="shared" si="6"/>
@@ -1613,7 +1617,7 @@
       <c r="E10" s="3"/>
       <c r="F10" s="4">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G10" s="4">
         <f t="shared" si="3"/>
@@ -1625,11 +1629,11 @@
       </c>
       <c r="I10" s="4">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="J10" s="4">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K10" s="7">
         <f t="shared" si="6"/>
@@ -1649,7 +1653,7 @@
       <c r="E11" s="3"/>
       <c r="F11" s="4">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G11" s="4">
         <f t="shared" si="3"/>
@@ -1661,11 +1665,11 @@
       </c>
       <c r="I11" s="4">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="J11" s="4">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K11" s="7">
         <f t="shared" si="6"/>
@@ -1685,7 +1689,7 @@
       <c r="E12" s="3"/>
       <c r="F12" s="4">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G12" s="4">
         <f t="shared" si="3"/>
@@ -1697,11 +1701,11 @@
       </c>
       <c r="I12" s="4">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="J12" s="4">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K12" s="7">
         <f t="shared" si="6"/>
@@ -1721,7 +1725,7 @@
       <c r="E13" s="3"/>
       <c r="F13" s="4">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G13" s="4">
         <f t="shared" si="3"/>
@@ -1733,11 +1737,11 @@
       </c>
       <c r="I13" s="4">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="J13" s="4">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K13" s="7">
         <f t="shared" si="6"/>
@@ -1757,7 +1761,7 @@
       <c r="E14" s="3"/>
       <c r="F14" s="4">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G14" s="4">
         <f t="shared" si="3"/>
@@ -1769,11 +1773,11 @@
       </c>
       <c r="I14" s="4">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="J14" s="4">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K14" s="7">
         <f t="shared" si="6"/>
@@ -1793,7 +1797,7 @@
       <c r="E15" s="3"/>
       <c r="F15" s="4">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G15" s="4">
         <f t="shared" si="3"/>
@@ -1805,11 +1809,11 @@
       </c>
       <c r="I15" s="4">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="J15" s="4">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K15" s="7">
         <f t="shared" si="6"/>
@@ -1829,7 +1833,7 @@
       <c r="E16" s="3"/>
       <c r="F16" s="4">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G16" s="4">
         <f t="shared" si="3"/>
@@ -1841,11 +1845,11 @@
       </c>
       <c r="I16" s="4">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="J16" s="4">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K16" s="7">
         <f t="shared" si="6"/>
@@ -1865,7 +1869,7 @@
       <c r="E17" s="3"/>
       <c r="F17" s="4">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G17" s="4">
         <f t="shared" si="3"/>
@@ -1877,11 +1881,11 @@
       </c>
       <c r="I17" s="4">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="J17" s="4">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K17" s="7">
         <f t="shared" si="6"/>
@@ -1901,7 +1905,7 @@
       <c r="E18" s="3"/>
       <c r="F18" s="4">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G18" s="4">
         <f t="shared" si="3"/>
@@ -1913,11 +1917,11 @@
       </c>
       <c r="I18" s="4">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="J18" s="4">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K18" s="7">
         <f t="shared" si="6"/>
@@ -1937,7 +1941,7 @@
       <c r="E19" s="3"/>
       <c r="F19" s="4">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G19" s="4">
         <f t="shared" si="3"/>
@@ -1949,11 +1953,11 @@
       </c>
       <c r="I19" s="4">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="J19" s="4">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K19" s="7">
         <f t="shared" si="6"/>
@@ -1973,7 +1977,7 @@
       <c r="E20" s="3"/>
       <c r="F20" s="4">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G20" s="4">
         <f t="shared" si="3"/>
@@ -1985,11 +1989,11 @@
       </c>
       <c r="I20" s="4">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="J20" s="4">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K20" s="7">
         <f t="shared" si="6"/>
@@ -2009,7 +2013,7 @@
       <c r="E21" s="3"/>
       <c r="F21" s="4">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G21" s="4">
         <f t="shared" si="3"/>
@@ -2021,11 +2025,11 @@
       </c>
       <c r="I21" s="4">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="J21" s="4">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K21" s="7">
         <f t="shared" si="6"/>
@@ -2045,7 +2049,7 @@
       <c r="E22" s="3"/>
       <c r="F22" s="4">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G22" s="4">
         <f t="shared" si="3"/>
@@ -2057,11 +2061,11 @@
       </c>
       <c r="I22" s="4">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="J22" s="4">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K22" s="7">
         <f t="shared" si="6"/>
@@ -2081,7 +2085,7 @@
       <c r="E23" s="3"/>
       <c r="F23" s="4">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G23" s="4">
         <f t="shared" si="3"/>
@@ -2093,11 +2097,11 @@
       </c>
       <c r="I23" s="4">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="J23" s="4">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K23" s="7">
         <f t="shared" si="6"/>
@@ -2117,7 +2121,7 @@
       <c r="E24" s="3"/>
       <c r="F24" s="4">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G24" s="4">
         <f t="shared" si="3"/>
@@ -2129,11 +2133,11 @@
       </c>
       <c r="I24" s="4">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="J24" s="4">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K24" s="7">
         <f t="shared" si="6"/>
@@ -2153,7 +2157,7 @@
       <c r="E25" s="3"/>
       <c r="F25" s="4">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G25" s="4">
         <f t="shared" si="3"/>
@@ -2165,11 +2169,11 @@
       </c>
       <c r="I25" s="4">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="J25" s="4">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K25" s="7">
         <f t="shared" si="6"/>
@@ -2189,7 +2193,7 @@
       <c r="E26" s="3"/>
       <c r="F26" s="4">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G26" s="4">
         <f t="shared" si="3"/>
@@ -2201,11 +2205,11 @@
       </c>
       <c r="I26" s="4">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="J26" s="4">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K26" s="7">
         <f t="shared" si="6"/>
@@ -2225,7 +2229,7 @@
       <c r="E27" s="3"/>
       <c r="F27" s="4">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G27" s="4">
         <f t="shared" si="3"/>
@@ -2237,11 +2241,11 @@
       </c>
       <c r="I27" s="4">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="J27" s="4">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K27" s="7">
         <f t="shared" si="6"/>
@@ -2261,7 +2265,7 @@
       <c r="E28" s="3"/>
       <c r="F28" s="4">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G28" s="4">
         <f t="shared" si="3"/>
@@ -2273,11 +2277,11 @@
       </c>
       <c r="I28" s="4">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="J28" s="4">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K28" s="7">
         <f t="shared" si="6"/>
@@ -2297,7 +2301,7 @@
       <c r="E29" s="3"/>
       <c r="F29" s="4">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G29" s="4">
         <f t="shared" si="3"/>
@@ -2309,11 +2313,11 @@
       </c>
       <c r="I29" s="4">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="J29" s="4">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K29" s="7">
         <f t="shared" si="6"/>
@@ -2333,7 +2337,7 @@
       <c r="E30" s="3"/>
       <c r="F30" s="4">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G30" s="4">
         <f t="shared" si="3"/>
@@ -2345,11 +2349,11 @@
       </c>
       <c r="I30" s="4">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="J30" s="4">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K30" s="7">
         <f t="shared" si="6"/>
@@ -2369,7 +2373,7 @@
       <c r="E31" s="3"/>
       <c r="F31" s="4">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G31" s="4">
         <f t="shared" si="3"/>
@@ -2381,11 +2385,11 @@
       </c>
       <c r="I31" s="4">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="J31" s="4">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K31" s="7">
         <f t="shared" si="6"/>
@@ -2405,7 +2409,7 @@
       <c r="E32" s="3"/>
       <c r="F32" s="4">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G32" s="4">
         <f t="shared" si="3"/>
@@ -2417,11 +2421,11 @@
       </c>
       <c r="I32" s="4">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="J32" s="4">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K32" s="7">
         <f t="shared" si="6"/>
@@ -2441,7 +2445,7 @@
       <c r="E33" s="3"/>
       <c r="F33" s="4">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G33" s="4">
         <f t="shared" si="3"/>
@@ -2453,11 +2457,11 @@
       </c>
       <c r="I33" s="4">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="J33" s="4">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K33" s="7">
         <f t="shared" si="6"/>
@@ -2477,7 +2481,7 @@
       <c r="E34" s="3"/>
       <c r="F34" s="4">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G34" s="4">
         <f t="shared" si="3"/>
@@ -2489,11 +2493,11 @@
       </c>
       <c r="I34" s="4">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="J34" s="4">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K34" s="7">
         <f t="shared" si="6"/>
@@ -2513,7 +2517,7 @@
       <c r="E35" s="3"/>
       <c r="F35" s="4">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G35" s="4">
         <f t="shared" si="3"/>
@@ -2525,11 +2529,11 @@
       </c>
       <c r="I35" s="4">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="J35" s="4">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K35" s="7">
         <f t="shared" si="6"/>
@@ -2549,7 +2553,7 @@
       <c r="E36" s="3"/>
       <c r="F36" s="4">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G36" s="4">
         <f t="shared" si="3"/>
@@ -2561,11 +2565,11 @@
       </c>
       <c r="I36" s="4">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="J36" s="4">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K36" s="7">
         <f t="shared" si="6"/>
@@ -2585,7 +2589,7 @@
       <c r="E37" s="3"/>
       <c r="F37" s="4">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G37" s="4">
         <f t="shared" si="3"/>
@@ -2597,11 +2601,11 @@
       </c>
       <c r="I37" s="4">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="J37" s="4">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K37" s="7">
         <f t="shared" si="6"/>
@@ -2621,7 +2625,7 @@
       <c r="E38" s="3"/>
       <c r="F38" s="4">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G38" s="4">
         <f t="shared" si="3"/>
@@ -2633,11 +2637,11 @@
       </c>
       <c r="I38" s="4">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="J38" s="4">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K38" s="7">
         <f t="shared" si="6"/>
@@ -2657,7 +2661,7 @@
       <c r="E39" s="3"/>
       <c r="F39" s="4">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G39" s="4">
         <f t="shared" si="3"/>
@@ -2669,11 +2673,11 @@
       </c>
       <c r="I39" s="4">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="J39" s="4">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K39" s="7">
         <f t="shared" si="6"/>
@@ -2693,7 +2697,7 @@
       <c r="E40" s="3"/>
       <c r="F40" s="4">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G40" s="4">
         <f t="shared" si="3"/>
@@ -2705,11 +2709,11 @@
       </c>
       <c r="I40" s="4">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="J40" s="4">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K40" s="7">
         <f t="shared" si="6"/>
@@ -2729,7 +2733,7 @@
       <c r="E41" s="3"/>
       <c r="F41" s="4">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G41" s="4">
         <f t="shared" si="3"/>
@@ -2741,11 +2745,11 @@
       </c>
       <c r="I41" s="4">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="J41" s="4">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K41" s="7">
         <f t="shared" si="6"/>
@@ -2765,7 +2769,7 @@
       <c r="E42" s="3"/>
       <c r="F42" s="4">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G42" s="4">
         <f t="shared" si="3"/>
@@ -2777,11 +2781,11 @@
       </c>
       <c r="I42" s="4">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="J42" s="4">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K42" s="7">
         <f t="shared" si="6"/>
@@ -2801,7 +2805,7 @@
       <c r="E43" s="3"/>
       <c r="F43" s="4">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G43" s="4">
         <f t="shared" si="3"/>
@@ -2813,11 +2817,11 @@
       </c>
       <c r="I43" s="4">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="J43" s="4">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K43" s="7">
         <f t="shared" si="6"/>
@@ -2837,7 +2841,7 @@
       <c r="E44" s="3"/>
       <c r="F44" s="4">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G44" s="4">
         <f t="shared" si="3"/>
@@ -2849,11 +2853,11 @@
       </c>
       <c r="I44" s="4">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="J44" s="4">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K44" s="7">
         <f t="shared" si="6"/>
@@ -2873,7 +2877,7 @@
       <c r="E45" s="3"/>
       <c r="F45" s="4">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G45" s="4">
         <f t="shared" si="3"/>
@@ -2885,11 +2889,11 @@
       </c>
       <c r="I45" s="4">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="J45" s="4">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K45" s="7">
         <f t="shared" si="6"/>
@@ -2909,7 +2913,7 @@
       <c r="E46" s="3"/>
       <c r="F46" s="4">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G46" s="4">
         <f t="shared" si="3"/>
@@ -2921,11 +2925,11 @@
       </c>
       <c r="I46" s="4">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="J46" s="4">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K46" s="7">
         <f t="shared" si="6"/>
@@ -2945,7 +2949,7 @@
       <c r="E47" s="3"/>
       <c r="F47" s="4">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G47" s="4">
         <f t="shared" si="3"/>
@@ -2957,11 +2961,11 @@
       </c>
       <c r="I47" s="4">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="J47" s="4">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K47" s="7">
         <f t="shared" si="6"/>
@@ -2981,7 +2985,7 @@
       <c r="E48" s="3"/>
       <c r="F48" s="4">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G48" s="4">
         <f t="shared" si="3"/>
@@ -2993,11 +2997,11 @@
       </c>
       <c r="I48" s="4">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="J48" s="4">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K48" s="7">
         <f t="shared" si="6"/>
@@ -3008,7 +3012,7 @@
       <c r="A49" s="8"/>
       <c r="B49" s="9">
         <f>SUM(B3:B27)</f>
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C49" s="9"/>
       <c r="D49" s="9">
@@ -3017,7 +3021,7 @@
       </c>
       <c r="E49" s="9">
         <f>AVERAGE(E3:E48)</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F49" s="9"/>
       <c r="G49" s="9"/>
@@ -3045,7 +3049,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="H8" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="H1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
Zwischencommit Admin-Area (neue Admins können hinzugefügt werden, Adminbereich ist geschützt, neue Metadaten können hinzugefügt werden)
</commit_message>
<xml_diff>
--- a/01_Planning/ProductBurndown.xlsx
+++ b/01_Planning/ProductBurndown.xlsx
@@ -512,121 +512,121 @@
                   <c:v>11.344827586206897</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11.103448275862069</c:v>
+                  <c:v>10.344827586206897</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10.827586206896552</c:v>
+                  <c:v>9.5670498084291182</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10.551724137931034</c:v>
+                  <c:v>9.2707535121328224</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10.275862068965516</c:v>
+                  <c:v>8.9744572158365266</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>10.275862068965516</c:v>
+                  <c:v>8.9744572158365266</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>10.275862068965516</c:v>
+                  <c:v>8.9744572158365266</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>10.275862068965516</c:v>
+                  <c:v>8.9744572158365266</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>10.275862068965516</c:v>
+                  <c:v>8.9744572158365266</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>10.275862068965516</c:v>
+                  <c:v>8.9744572158365266</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>10.275862068965516</c:v>
+                  <c:v>8.9744572158365266</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>10.275862068965516</c:v>
+                  <c:v>8.9744572158365266</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>10.275862068965516</c:v>
+                  <c:v>8.9744572158365266</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>10.275862068965516</c:v>
+                  <c:v>8.9744572158365266</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>9.9999999999999982</c:v>
+                  <c:v>8.6781609195402307</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>9.7241379310344804</c:v>
+                  <c:v>8.3818646232439349</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>9.4482758620689626</c:v>
+                  <c:v>8.0855683269476391</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>9.1724137931034448</c:v>
+                  <c:v>7.7892720306513432</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>8.8965517241379271</c:v>
+                  <c:v>7.4929757343550474</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>8.6206896551724093</c:v>
+                  <c:v>7.1966794380587515</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>8.3448275862068915</c:v>
+                  <c:v>6.9003831417624557</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>8.0689655172413737</c:v>
+                  <c:v>6.6040868454661599</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>7.7931034482758568</c:v>
+                  <c:v>6.307790549169864</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>7.5172413793103399</c:v>
+                  <c:v>6.0114942528735682</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>7.241379310344823</c:v>
+                  <c:v>5.7151979565772724</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>6.9655172413793061</c:v>
+                  <c:v>5.4189016602809765</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>6.6896551724137892</c:v>
+                  <c:v>5.1226053639846807</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>6.4137931034482722</c:v>
+                  <c:v>4.8263090676883849</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>6.1379310344827553</c:v>
+                  <c:v>4.530012771392089</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>5.8620689655172384</c:v>
+                  <c:v>4.2337164750957932</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>5.5862068965517215</c:v>
+                  <c:v>3.9374201787994969</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>5.3103448275862046</c:v>
+                  <c:v>3.6411238825032006</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>5.0344827586206877</c:v>
+                  <c:v>3.3448275862069043</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>4.7586206896551708</c:v>
+                  <c:v>3.0485312899106081</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>4.4827586206896539</c:v>
+                  <c:v>2.7522349936143118</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>4.206896551724137</c:v>
+                  <c:v>2.4559386973180155</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>3.9310344827586197</c:v>
+                  <c:v>2.1596424010217192</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>3.6551724137931023</c:v>
+                  <c:v>1.8633461047254229</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>3.379310344827585</c:v>
+                  <c:v>1.5670498084291267</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>3.1034482758620676</c:v>
+                  <c:v>1.2707535121328304</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -642,11 +642,11 @@
         </c:dLbls>
         <c:gapWidth val="40"/>
         <c:overlap val="-10"/>
-        <c:axId val="401519072"/>
-        <c:axId val="401524168"/>
+        <c:axId val="392204488"/>
+        <c:axId val="392205664"/>
       </c:barChart>
       <c:dateAx>
-        <c:axId val="401519072"/>
+        <c:axId val="392204488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -685,14 +685,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="401524168"/>
+        <c:crossAx val="392205664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="401524168"/>
+        <c:axId val="392205664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -738,7 +738,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="401519072"/>
+        <c:crossAx val="392204488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="25"/>
@@ -1276,7 +1276,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomRight" activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1628,7 +1628,9 @@
       <c r="D10" s="3">
         <v>1</v>
       </c>
-      <c r="E10" s="3"/>
+      <c r="E10" s="3">
+        <v>6</v>
+      </c>
       <c r="F10" s="4">
         <f t="shared" si="2"/>
         <v>11.344827586206897</v>
@@ -1647,11 +1649,11 @@
       </c>
       <c r="J10" s="4">
         <f t="shared" si="5"/>
-        <v>11.103448275862069</v>
+        <v>10.344827586206897</v>
       </c>
       <c r="K10" s="7">
         <f t="shared" si="6"/>
-        <v>3.4482758620689655E-2</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -1660,14 +1662,14 @@
         <v>41447</v>
       </c>
       <c r="B11" s="3">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="4">
         <f t="shared" si="2"/>
-        <v>11.103448275862069</v>
+        <v>10.344827586206897</v>
       </c>
       <c r="G11" s="4">
         <f t="shared" si="3"/>
@@ -1679,15 +1681,15 @@
       </c>
       <c r="I11" s="4">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="J11" s="4">
         <f t="shared" si="5"/>
-        <v>10.827586206896552</v>
+        <v>9.5670498084291182</v>
       </c>
       <c r="K11" s="7">
         <f t="shared" si="6"/>
-        <v>3.4482758620689655E-2</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -1703,7 +1705,7 @@
       <c r="E12" s="3"/>
       <c r="F12" s="4">
         <f t="shared" si="2"/>
-        <v>10.827586206896552</v>
+        <v>9.5670498084291182</v>
       </c>
       <c r="G12" s="4">
         <f t="shared" si="3"/>
@@ -1715,15 +1717,15 @@
       </c>
       <c r="I12" s="4">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="J12" s="4">
         <f t="shared" si="5"/>
-        <v>10.551724137931034</v>
+        <v>9.2707535121328224</v>
       </c>
       <c r="K12" s="7">
         <f t="shared" si="6"/>
-        <v>3.4482758620689655E-2</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -1739,7 +1741,7 @@
       <c r="E13" s="3"/>
       <c r="F13" s="4">
         <f t="shared" si="2"/>
-        <v>10.551724137931034</v>
+        <v>9.2707535121328224</v>
       </c>
       <c r="G13" s="4">
         <f t="shared" si="3"/>
@@ -1751,15 +1753,15 @@
       </c>
       <c r="I13" s="4">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="J13" s="4">
         <f t="shared" si="5"/>
-        <v>10.275862068965516</v>
+        <v>8.9744572158365266</v>
       </c>
       <c r="K13" s="7">
         <f t="shared" si="6"/>
-        <v>3.4482758620689655E-2</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -1775,7 +1777,7 @@
       <c r="E14" s="3"/>
       <c r="F14" s="4">
         <f t="shared" si="2"/>
-        <v>10.275862068965516</v>
+        <v>8.9744572158365266</v>
       </c>
       <c r="G14" s="4">
         <f t="shared" si="3"/>
@@ -1787,15 +1789,15 @@
       </c>
       <c r="I14" s="4">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="J14" s="4">
         <f t="shared" si="5"/>
-        <v>10.275862068965516</v>
+        <v>8.9744572158365266</v>
       </c>
       <c r="K14" s="7">
         <f t="shared" si="6"/>
-        <v>3.4482758620689655E-2</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -1811,7 +1813,7 @@
       <c r="E15" s="3"/>
       <c r="F15" s="4">
         <f t="shared" si="2"/>
-        <v>10.275862068965516</v>
+        <v>8.9744572158365266</v>
       </c>
       <c r="G15" s="4">
         <f t="shared" si="3"/>
@@ -1823,15 +1825,15 @@
       </c>
       <c r="I15" s="4">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="J15" s="4">
         <f t="shared" si="5"/>
-        <v>10.275862068965516</v>
+        <v>8.9744572158365266</v>
       </c>
       <c r="K15" s="7">
         <f t="shared" si="6"/>
-        <v>3.4482758620689655E-2</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -1847,7 +1849,7 @@
       <c r="E16" s="3"/>
       <c r="F16" s="4">
         <f t="shared" si="2"/>
-        <v>10.275862068965516</v>
+        <v>8.9744572158365266</v>
       </c>
       <c r="G16" s="4">
         <f t="shared" si="3"/>
@@ -1859,15 +1861,15 @@
       </c>
       <c r="I16" s="4">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="J16" s="4">
         <f t="shared" si="5"/>
-        <v>10.275862068965516</v>
+        <v>8.9744572158365266</v>
       </c>
       <c r="K16" s="7">
         <f t="shared" si="6"/>
-        <v>3.4482758620689655E-2</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -1883,7 +1885,7 @@
       <c r="E17" s="3"/>
       <c r="F17" s="4">
         <f t="shared" si="2"/>
-        <v>10.275862068965516</v>
+        <v>8.9744572158365266</v>
       </c>
       <c r="G17" s="4">
         <f t="shared" si="3"/>
@@ -1895,15 +1897,15 @@
       </c>
       <c r="I17" s="4">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="J17" s="4">
         <f t="shared" si="5"/>
-        <v>10.275862068965516</v>
+        <v>8.9744572158365266</v>
       </c>
       <c r="K17" s="7">
         <f t="shared" si="6"/>
-        <v>3.4482758620689655E-2</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -1919,7 +1921,7 @@
       <c r="E18" s="3"/>
       <c r="F18" s="4">
         <f t="shared" si="2"/>
-        <v>10.275862068965516</v>
+        <v>8.9744572158365266</v>
       </c>
       <c r="G18" s="4">
         <f t="shared" si="3"/>
@@ -1931,15 +1933,15 @@
       </c>
       <c r="I18" s="4">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="J18" s="4">
         <f t="shared" si="5"/>
-        <v>10.275862068965516</v>
+        <v>8.9744572158365266</v>
       </c>
       <c r="K18" s="7">
         <f t="shared" si="6"/>
-        <v>3.4482758620689655E-2</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -1955,7 +1957,7 @@
       <c r="E19" s="3"/>
       <c r="F19" s="4">
         <f t="shared" si="2"/>
-        <v>10.275862068965516</v>
+        <v>8.9744572158365266</v>
       </c>
       <c r="G19" s="4">
         <f t="shared" si="3"/>
@@ -1967,15 +1969,15 @@
       </c>
       <c r="I19" s="4">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="J19" s="4">
         <f t="shared" si="5"/>
-        <v>10.275862068965516</v>
+        <v>8.9744572158365266</v>
       </c>
       <c r="K19" s="7">
         <f t="shared" si="6"/>
-        <v>3.4482758620689655E-2</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -1991,7 +1993,7 @@
       <c r="E20" s="3"/>
       <c r="F20" s="4">
         <f t="shared" si="2"/>
-        <v>10.275862068965516</v>
+        <v>8.9744572158365266</v>
       </c>
       <c r="G20" s="4">
         <f t="shared" si="3"/>
@@ -2003,15 +2005,15 @@
       </c>
       <c r="I20" s="4">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="J20" s="4">
         <f t="shared" si="5"/>
-        <v>10.275862068965516</v>
+        <v>8.9744572158365266</v>
       </c>
       <c r="K20" s="7">
         <f t="shared" si="6"/>
-        <v>3.4482758620689655E-2</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2027,7 +2029,7 @@
       <c r="E21" s="3"/>
       <c r="F21" s="4">
         <f t="shared" si="2"/>
-        <v>10.275862068965516</v>
+        <v>8.9744572158365266</v>
       </c>
       <c r="G21" s="4">
         <f t="shared" si="3"/>
@@ -2039,15 +2041,15 @@
       </c>
       <c r="I21" s="4">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="J21" s="4">
         <f t="shared" si="5"/>
-        <v>10.275862068965516</v>
+        <v>8.9744572158365266</v>
       </c>
       <c r="K21" s="7">
         <f t="shared" si="6"/>
-        <v>3.4482758620689655E-2</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2063,7 +2065,7 @@
       <c r="E22" s="3"/>
       <c r="F22" s="4">
         <f t="shared" si="2"/>
-        <v>10.275862068965516</v>
+        <v>8.9744572158365266</v>
       </c>
       <c r="G22" s="4">
         <f t="shared" si="3"/>
@@ -2075,15 +2077,15 @@
       </c>
       <c r="I22" s="4">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="J22" s="4">
         <f t="shared" si="5"/>
-        <v>10.275862068965516</v>
+        <v>8.9744572158365266</v>
       </c>
       <c r="K22" s="7">
         <f t="shared" si="6"/>
-        <v>3.4482758620689655E-2</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2099,7 +2101,7 @@
       <c r="E23" s="3"/>
       <c r="F23" s="4">
         <f t="shared" si="2"/>
-        <v>10.275862068965516</v>
+        <v>8.9744572158365266</v>
       </c>
       <c r="G23" s="4">
         <f t="shared" si="3"/>
@@ -2111,15 +2113,15 @@
       </c>
       <c r="I23" s="4">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="J23" s="4">
         <f t="shared" si="5"/>
-        <v>9.9999999999999982</v>
+        <v>8.6781609195402307</v>
       </c>
       <c r="K23" s="7">
         <f t="shared" si="6"/>
-        <v>3.4482758620689655E-2</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2135,7 +2137,7 @@
       <c r="E24" s="3"/>
       <c r="F24" s="4">
         <f t="shared" si="2"/>
-        <v>9.9999999999999982</v>
+        <v>8.6781609195402307</v>
       </c>
       <c r="G24" s="4">
         <f t="shared" si="3"/>
@@ -2147,15 +2149,15 @@
       </c>
       <c r="I24" s="4">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="J24" s="4">
         <f t="shared" si="5"/>
-        <v>9.7241379310344804</v>
+        <v>8.3818646232439349</v>
       </c>
       <c r="K24" s="7">
         <f t="shared" si="6"/>
-        <v>3.4482758620689655E-2</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2171,7 +2173,7 @@
       <c r="E25" s="3"/>
       <c r="F25" s="4">
         <f t="shared" si="2"/>
-        <v>9.7241379310344804</v>
+        <v>8.3818646232439349</v>
       </c>
       <c r="G25" s="4">
         <f t="shared" si="3"/>
@@ -2183,15 +2185,15 @@
       </c>
       <c r="I25" s="4">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="J25" s="4">
         <f t="shared" si="5"/>
-        <v>9.4482758620689626</v>
+        <v>8.0855683269476391</v>
       </c>
       <c r="K25" s="7">
         <f t="shared" si="6"/>
-        <v>3.4482758620689655E-2</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2207,7 +2209,7 @@
       <c r="E26" s="3"/>
       <c r="F26" s="4">
         <f t="shared" si="2"/>
-        <v>9.4482758620689626</v>
+        <v>8.0855683269476391</v>
       </c>
       <c r="G26" s="4">
         <f t="shared" si="3"/>
@@ -2219,15 +2221,15 @@
       </c>
       <c r="I26" s="4">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="J26" s="4">
         <f t="shared" si="5"/>
-        <v>9.1724137931034448</v>
+        <v>7.7892720306513432</v>
       </c>
       <c r="K26" s="7">
         <f t="shared" si="6"/>
-        <v>3.4482758620689655E-2</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2243,7 +2245,7 @@
       <c r="E27" s="3"/>
       <c r="F27" s="4">
         <f t="shared" si="2"/>
-        <v>9.1724137931034448</v>
+        <v>7.7892720306513432</v>
       </c>
       <c r="G27" s="4">
         <f t="shared" si="3"/>
@@ -2255,15 +2257,15 @@
       </c>
       <c r="I27" s="4">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="J27" s="4">
         <f t="shared" si="5"/>
-        <v>8.8965517241379271</v>
+        <v>7.4929757343550474</v>
       </c>
       <c r="K27" s="7">
         <f t="shared" si="6"/>
-        <v>3.4482758620689655E-2</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2279,7 +2281,7 @@
       <c r="E28" s="3"/>
       <c r="F28" s="4">
         <f t="shared" si="2"/>
-        <v>8.8965517241379271</v>
+        <v>7.4929757343550474</v>
       </c>
       <c r="G28" s="4">
         <f t="shared" si="3"/>
@@ -2291,15 +2293,15 @@
       </c>
       <c r="I28" s="4">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="J28" s="4">
         <f t="shared" si="5"/>
-        <v>8.6206896551724093</v>
+        <v>7.1966794380587515</v>
       </c>
       <c r="K28" s="7">
         <f t="shared" si="6"/>
-        <v>3.4482758620689655E-2</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2315,7 +2317,7 @@
       <c r="E29" s="3"/>
       <c r="F29" s="4">
         <f t="shared" si="2"/>
-        <v>8.6206896551724093</v>
+        <v>7.1966794380587515</v>
       </c>
       <c r="G29" s="4">
         <f t="shared" si="3"/>
@@ -2327,15 +2329,15 @@
       </c>
       <c r="I29" s="4">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="J29" s="4">
         <f t="shared" si="5"/>
-        <v>8.3448275862068915</v>
+        <v>6.9003831417624557</v>
       </c>
       <c r="K29" s="7">
         <f t="shared" si="6"/>
-        <v>3.4482758620689655E-2</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2351,7 +2353,7 @@
       <c r="E30" s="3"/>
       <c r="F30" s="4">
         <f t="shared" si="2"/>
-        <v>8.3448275862068915</v>
+        <v>6.9003831417624557</v>
       </c>
       <c r="G30" s="4">
         <f t="shared" si="3"/>
@@ -2363,15 +2365,15 @@
       </c>
       <c r="I30" s="4">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="J30" s="4">
         <f t="shared" si="5"/>
-        <v>8.0689655172413737</v>
+        <v>6.6040868454661599</v>
       </c>
       <c r="K30" s="7">
         <f t="shared" si="6"/>
-        <v>3.4482758620689655E-2</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2387,7 +2389,7 @@
       <c r="E31" s="3"/>
       <c r="F31" s="4">
         <f t="shared" si="2"/>
-        <v>8.0689655172413737</v>
+        <v>6.6040868454661599</v>
       </c>
       <c r="G31" s="4">
         <f t="shared" si="3"/>
@@ -2399,15 +2401,15 @@
       </c>
       <c r="I31" s="4">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="J31" s="4">
         <f t="shared" si="5"/>
-        <v>7.7931034482758568</v>
+        <v>6.307790549169864</v>
       </c>
       <c r="K31" s="7">
         <f t="shared" si="6"/>
-        <v>3.4482758620689655E-2</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2423,7 +2425,7 @@
       <c r="E32" s="3"/>
       <c r="F32" s="4">
         <f t="shared" si="2"/>
-        <v>7.7931034482758568</v>
+        <v>6.307790549169864</v>
       </c>
       <c r="G32" s="4">
         <f t="shared" si="3"/>
@@ -2435,15 +2437,15 @@
       </c>
       <c r="I32" s="4">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="J32" s="4">
         <f t="shared" si="5"/>
-        <v>7.5172413793103399</v>
+        <v>6.0114942528735682</v>
       </c>
       <c r="K32" s="7">
         <f t="shared" si="6"/>
-        <v>3.4482758620689655E-2</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2459,7 +2461,7 @@
       <c r="E33" s="3"/>
       <c r="F33" s="4">
         <f t="shared" si="2"/>
-        <v>7.5172413793103399</v>
+        <v>6.0114942528735682</v>
       </c>
       <c r="G33" s="4">
         <f t="shared" si="3"/>
@@ -2471,15 +2473,15 @@
       </c>
       <c r="I33" s="4">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="J33" s="4">
         <f t="shared" si="5"/>
-        <v>7.241379310344823</v>
+        <v>5.7151979565772724</v>
       </c>
       <c r="K33" s="7">
         <f t="shared" si="6"/>
-        <v>3.4482758620689655E-2</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2495,7 +2497,7 @@
       <c r="E34" s="3"/>
       <c r="F34" s="4">
         <f t="shared" si="2"/>
-        <v>7.241379310344823</v>
+        <v>5.7151979565772724</v>
       </c>
       <c r="G34" s="4">
         <f t="shared" si="3"/>
@@ -2507,15 +2509,15 @@
       </c>
       <c r="I34" s="4">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="J34" s="4">
         <f t="shared" si="5"/>
-        <v>6.9655172413793061</v>
+        <v>5.4189016602809765</v>
       </c>
       <c r="K34" s="7">
         <f t="shared" si="6"/>
-        <v>3.4482758620689655E-2</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2531,7 +2533,7 @@
       <c r="E35" s="3"/>
       <c r="F35" s="4">
         <f t="shared" si="2"/>
-        <v>6.9655172413793061</v>
+        <v>5.4189016602809765</v>
       </c>
       <c r="G35" s="4">
         <f t="shared" si="3"/>
@@ -2543,15 +2545,15 @@
       </c>
       <c r="I35" s="4">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="J35" s="4">
         <f t="shared" si="5"/>
-        <v>6.6896551724137892</v>
+        <v>5.1226053639846807</v>
       </c>
       <c r="K35" s="7">
         <f t="shared" si="6"/>
-        <v>3.4482758620689655E-2</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2567,7 +2569,7 @@
       <c r="E36" s="3"/>
       <c r="F36" s="4">
         <f t="shared" si="2"/>
-        <v>6.6896551724137892</v>
+        <v>5.1226053639846807</v>
       </c>
       <c r="G36" s="4">
         <f t="shared" si="3"/>
@@ -2579,15 +2581,15 @@
       </c>
       <c r="I36" s="4">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="J36" s="4">
         <f t="shared" si="5"/>
-        <v>6.4137931034482722</v>
+        <v>4.8263090676883849</v>
       </c>
       <c r="K36" s="7">
         <f t="shared" si="6"/>
-        <v>3.4482758620689655E-2</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2603,7 +2605,7 @@
       <c r="E37" s="3"/>
       <c r="F37" s="4">
         <f t="shared" si="2"/>
-        <v>6.4137931034482722</v>
+        <v>4.8263090676883849</v>
       </c>
       <c r="G37" s="4">
         <f t="shared" si="3"/>
@@ -2615,15 +2617,15 @@
       </c>
       <c r="I37" s="4">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="J37" s="4">
         <f t="shared" si="5"/>
-        <v>6.1379310344827553</v>
+        <v>4.530012771392089</v>
       </c>
       <c r="K37" s="7">
         <f t="shared" si="6"/>
-        <v>3.4482758620689655E-2</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2639,7 +2641,7 @@
       <c r="E38" s="3"/>
       <c r="F38" s="4">
         <f t="shared" si="2"/>
-        <v>6.1379310344827553</v>
+        <v>4.530012771392089</v>
       </c>
       <c r="G38" s="4">
         <f t="shared" si="3"/>
@@ -2651,15 +2653,15 @@
       </c>
       <c r="I38" s="4">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="J38" s="4">
         <f t="shared" si="5"/>
-        <v>5.8620689655172384</v>
+        <v>4.2337164750957932</v>
       </c>
       <c r="K38" s="7">
         <f t="shared" si="6"/>
-        <v>3.4482758620689655E-2</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2675,7 +2677,7 @@
       <c r="E39" s="3"/>
       <c r="F39" s="4">
         <f t="shared" si="2"/>
-        <v>5.8620689655172384</v>
+        <v>4.2337164750957932</v>
       </c>
       <c r="G39" s="4">
         <f t="shared" si="3"/>
@@ -2687,15 +2689,15 @@
       </c>
       <c r="I39" s="4">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="J39" s="4">
         <f t="shared" si="5"/>
-        <v>5.5862068965517215</v>
+        <v>3.9374201787994969</v>
       </c>
       <c r="K39" s="7">
         <f t="shared" si="6"/>
-        <v>3.4482758620689655E-2</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2711,7 +2713,7 @@
       <c r="E40" s="3"/>
       <c r="F40" s="4">
         <f t="shared" si="2"/>
-        <v>5.5862068965517215</v>
+        <v>3.9374201787994969</v>
       </c>
       <c r="G40" s="4">
         <f t="shared" si="3"/>
@@ -2723,15 +2725,15 @@
       </c>
       <c r="I40" s="4">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="J40" s="4">
         <f t="shared" si="5"/>
-        <v>5.3103448275862046</v>
+        <v>3.6411238825032006</v>
       </c>
       <c r="K40" s="7">
         <f t="shared" si="6"/>
-        <v>3.4482758620689655E-2</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2747,7 +2749,7 @@
       <c r="E41" s="3"/>
       <c r="F41" s="4">
         <f t="shared" si="2"/>
-        <v>5.3103448275862046</v>
+        <v>3.6411238825032006</v>
       </c>
       <c r="G41" s="4">
         <f t="shared" si="3"/>
@@ -2759,15 +2761,15 @@
       </c>
       <c r="I41" s="4">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="J41" s="4">
         <f t="shared" si="5"/>
-        <v>5.0344827586206877</v>
+        <v>3.3448275862069043</v>
       </c>
       <c r="K41" s="7">
         <f t="shared" si="6"/>
-        <v>3.4482758620689655E-2</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2783,7 +2785,7 @@
       <c r="E42" s="3"/>
       <c r="F42" s="4">
         <f t="shared" si="2"/>
-        <v>5.0344827586206877</v>
+        <v>3.3448275862069043</v>
       </c>
       <c r="G42" s="4">
         <f t="shared" si="3"/>
@@ -2795,15 +2797,15 @@
       </c>
       <c r="I42" s="4">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="J42" s="4">
         <f t="shared" si="5"/>
-        <v>4.7586206896551708</v>
+        <v>3.0485312899106081</v>
       </c>
       <c r="K42" s="7">
         <f t="shared" si="6"/>
-        <v>3.4482758620689655E-2</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2819,7 +2821,7 @@
       <c r="E43" s="3"/>
       <c r="F43" s="4">
         <f t="shared" si="2"/>
-        <v>4.7586206896551708</v>
+        <v>3.0485312899106081</v>
       </c>
       <c r="G43" s="4">
         <f t="shared" si="3"/>
@@ -2831,15 +2833,15 @@
       </c>
       <c r="I43" s="4">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="J43" s="4">
         <f t="shared" si="5"/>
-        <v>4.4827586206896539</v>
+        <v>2.7522349936143118</v>
       </c>
       <c r="K43" s="7">
         <f t="shared" si="6"/>
-        <v>3.4482758620689655E-2</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2855,7 +2857,7 @@
       <c r="E44" s="3"/>
       <c r="F44" s="4">
         <f t="shared" si="2"/>
-        <v>4.4827586206896539</v>
+        <v>2.7522349936143118</v>
       </c>
       <c r="G44" s="4">
         <f t="shared" si="3"/>
@@ -2867,15 +2869,15 @@
       </c>
       <c r="I44" s="4">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="J44" s="4">
         <f t="shared" si="5"/>
-        <v>4.206896551724137</v>
+        <v>2.4559386973180155</v>
       </c>
       <c r="K44" s="7">
         <f t="shared" si="6"/>
-        <v>3.4482758620689655E-2</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2891,7 +2893,7 @@
       <c r="E45" s="3"/>
       <c r="F45" s="4">
         <f t="shared" si="2"/>
-        <v>4.206896551724137</v>
+        <v>2.4559386973180155</v>
       </c>
       <c r="G45" s="4">
         <f t="shared" si="3"/>
@@ -2903,15 +2905,15 @@
       </c>
       <c r="I45" s="4">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="J45" s="4">
         <f t="shared" si="5"/>
-        <v>3.9310344827586197</v>
+        <v>2.1596424010217192</v>
       </c>
       <c r="K45" s="7">
         <f t="shared" si="6"/>
-        <v>3.4482758620689655E-2</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2927,7 +2929,7 @@
       <c r="E46" s="3"/>
       <c r="F46" s="4">
         <f t="shared" si="2"/>
-        <v>3.9310344827586197</v>
+        <v>2.1596424010217192</v>
       </c>
       <c r="G46" s="4">
         <f t="shared" si="3"/>
@@ -2939,15 +2941,15 @@
       </c>
       <c r="I46" s="4">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="J46" s="4">
         <f t="shared" si="5"/>
-        <v>3.6551724137931023</v>
+        <v>1.8633461047254229</v>
       </c>
       <c r="K46" s="7">
         <f t="shared" si="6"/>
-        <v>3.4482758620689655E-2</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2963,7 +2965,7 @@
       <c r="E47" s="3"/>
       <c r="F47" s="4">
         <f t="shared" si="2"/>
-        <v>3.6551724137931023</v>
+        <v>1.8633461047254229</v>
       </c>
       <c r="G47" s="4">
         <f t="shared" si="3"/>
@@ -2975,15 +2977,15 @@
       </c>
       <c r="I47" s="4">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="J47" s="4">
         <f t="shared" si="5"/>
-        <v>3.379310344827585</v>
+        <v>1.5670498084291267</v>
       </c>
       <c r="K47" s="7">
         <f t="shared" si="6"/>
-        <v>3.4482758620689655E-2</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="20.65" customHeight="1" x14ac:dyDescent="0.2">
@@ -2999,7 +3001,7 @@
       <c r="E48" s="3"/>
       <c r="F48" s="4">
         <f t="shared" si="2"/>
-        <v>3.379310344827585</v>
+        <v>1.5670498084291267</v>
       </c>
       <c r="G48" s="4">
         <f t="shared" si="3"/>
@@ -3011,22 +3013,22 @@
       </c>
       <c r="I48" s="4">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="J48" s="4">
         <f t="shared" si="5"/>
-        <v>3.1034482758620676</v>
+        <v>1.2707535121328304</v>
       </c>
       <c r="K48" s="7">
         <f t="shared" si="6"/>
-        <v>3.4482758620689655E-2</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="49" spans="1:11" ht="20.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="8"/>
       <c r="B49" s="9">
         <f>SUM(B3:B27)</f>
-        <v>124</v>
+        <v>137</v>
       </c>
       <c r="C49" s="9"/>
       <c r="D49" s="9">
@@ -3035,7 +3037,7 @@
       </c>
       <c r="E49" s="9">
         <f>AVERAGE(E3:E48)</f>
-        <v>6.8571428571428568</v>
+        <v>6.75</v>
       </c>
       <c r="F49" s="9"/>
       <c r="G49" s="9"/>

</xml_diff>

<commit_message>
M-M Relationship Tutor Subject simplified; Statistics work
</commit_message>
<xml_diff>
--- a/01_Planning/ProductBurndown.xlsx
+++ b/01_Planning/ProductBurndown.xlsx
@@ -494,139 +494,139 @@
                   <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.625</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.75</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.75</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>11.724137931034482</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>12.482758620689655</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>12.344827586206897</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>11.344827586206897</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>10.567049808429118</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>10.270753512132822</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>9.9744572158365266</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>9.9744572158365266</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>9.9744572158365266</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>9.9744572158365266</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>9.9744572158365266</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>9.9744572158365266</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>9.9744572158365266</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>9.9744572158365266</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>9.9744572158365266</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>9.9744572158365266</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>9.4559386973180075</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0</c:v>
+                  <c:v>8.6411238825031926</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0</c:v>
+                  <c:v>8.3448275862068968</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3.4444444444444446</c:v>
+                  <c:v>12.900383141762452</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.4074074074074074</c:v>
+                  <c:v>12.641123882503193</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.3703703703703705</c:v>
+                  <c:v>12.344827586206897</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.33333333333333348</c:v>
+                  <c:v>12.048531289910601</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0</c:v>
+                  <c:v>11.752234993614305</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0</c:v>
+                  <c:v>11.455938697318009</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0</c:v>
+                  <c:v>11.159642401021713</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0</c:v>
+                  <c:v>10.863346104725418</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0</c:v>
+                  <c:v>10.567049808429122</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0</c:v>
+                  <c:v>10.270753512132826</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0</c:v>
+                  <c:v>9.9744572158365301</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0</c:v>
+                  <c:v>9.6781609195402343</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0</c:v>
+                  <c:v>9.3818646232439384</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0</c:v>
+                  <c:v>9.0855683269476426</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0</c:v>
+                  <c:v>8.7892720306513468</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0</c:v>
+                  <c:v>8.4929757343550509</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0</c:v>
+                  <c:v>8.1966794380587551</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0</c:v>
+                  <c:v>7.9003831417624593</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0</c:v>
+                  <c:v>7.6040868454661634</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0</c:v>
+                  <c:v>7.3077905491698676</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0</c:v>
+                  <c:v>7.0114942528735718</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0</c:v>
+                  <c:v>6.7151979565772759</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0</c:v>
+                  <c:v>6.4189016602809801</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -642,11 +642,11 @@
         </c:dLbls>
         <c:gapWidth val="40"/>
         <c:overlap val="-10"/>
-        <c:axId val="158255392"/>
-        <c:axId val="158256176"/>
+        <c:axId val="192915800"/>
+        <c:axId val="192909920"/>
       </c:barChart>
       <c:dateAx>
-        <c:axId val="158255392"/>
+        <c:axId val="192915800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -685,14 +685,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="158256176"/>
+        <c:crossAx val="192909920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="158256176"/>
+        <c:axId val="192909920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -738,7 +738,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="158255392"/>
+        <c:crossAx val="192915800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="25"/>
@@ -1204,7 +1204,7 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1243,7 +1243,7 @@
         <v>13</v>
       </c>
       <c r="B3" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C3" s="3">
         <v>0</v>
@@ -1273,10 +1273,10 @@
   <dimension ref="A1:IV49"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G17" sqref="G17"/>
+      <selection pane="bottomRight" activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1365,11 +1365,11 @@
       </c>
       <c r="G3" s="4">
         <f>'Sheet 1 - Initial'!B3</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H3" s="4">
         <f t="shared" ref="H3:H48" si="0">G3+D3</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I3" s="4">
         <f>'Sheet 1 - Initial'!C3</f>
@@ -1381,7 +1381,7 @@
       </c>
       <c r="K3" s="7">
         <f>IF(OR(ISBLANK(D3),ISBLANK(E3)),'Sheet 1 - Initial'!D3,H3/(I3+E3))</f>
-        <v>0.625</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -1403,11 +1403,11 @@
       </c>
       <c r="G4" s="4">
         <f t="shared" ref="G4:G48" si="3">H3</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H4" s="4">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I4" s="4">
         <f t="shared" ref="I4:I48" si="4">I3+E3</f>
@@ -1415,11 +1415,11 @@
       </c>
       <c r="J4" s="4">
         <f t="shared" ref="J4:J48" si="5">MAX(IF(OR(ISBLANK(D4),ISBLANK(E4)),F4-K3*B4,F4-D4),0)</f>
-        <v>8.625</v>
+        <v>13</v>
       </c>
       <c r="K4" s="7">
         <f t="shared" ref="K4:K48" si="6">IF(OR(ISBLANK(D4),ISBLANK(E4)),K3,H4/(I4+E4))</f>
-        <v>0.625</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -1437,15 +1437,15 @@
       </c>
       <c r="F5" s="4">
         <f t="shared" si="2"/>
-        <v>8.625</v>
+        <v>13</v>
       </c>
       <c r="G5" s="4">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H5" s="4">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I5" s="4">
         <f t="shared" si="4"/>
@@ -1453,11 +1453,11 @@
       </c>
       <c r="J5" s="4">
         <f t="shared" si="5"/>
-        <v>1.75</v>
+        <v>13</v>
       </c>
       <c r="K5" s="7">
         <f t="shared" si="6"/>
-        <v>0.625</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -1477,15 +1477,15 @@
       </c>
       <c r="F6" s="4">
         <f>J5+C6</f>
-        <v>1.75</v>
+        <v>13</v>
       </c>
       <c r="G6" s="4">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H6" s="4">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I6" s="4">
         <f t="shared" si="4"/>
@@ -1493,11 +1493,11 @@
       </c>
       <c r="J6" s="4">
         <f t="shared" si="5"/>
-        <v>0.75</v>
+        <v>12</v>
       </c>
       <c r="K6" s="7">
         <f t="shared" si="6"/>
-        <v>0.20689655172413793</v>
+        <v>3.4482758620689655E-2</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -1515,15 +1515,15 @@
       </c>
       <c r="F7" s="4">
         <f>J6+C7</f>
-        <v>0.75</v>
+        <v>12</v>
       </c>
       <c r="G7" s="4">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H7" s="4">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I7" s="4">
         <f t="shared" si="4"/>
@@ -1531,11 +1531,11 @@
       </c>
       <c r="J7" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>11.724137931034482</v>
       </c>
       <c r="K7" s="7">
         <f t="shared" si="6"/>
-        <v>0.20689655172413793</v>
+        <v>3.4482758620689655E-2</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -1555,15 +1555,15 @@
       </c>
       <c r="F8" s="4">
         <f t="shared" si="2"/>
+        <v>12.724137931034482</v>
+      </c>
+      <c r="G8" s="4">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="G8" s="4">
-        <f t="shared" si="3"/>
-        <v>6</v>
-      </c>
       <c r="H8" s="4">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I8" s="4">
         <f t="shared" si="4"/>
@@ -1571,11 +1571,11 @@
       </c>
       <c r="J8" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>12.482758620689655</v>
       </c>
       <c r="K8" s="7">
         <f t="shared" si="6"/>
-        <v>0.20689655172413793</v>
+        <v>3.4482758620689655E-2</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -1593,15 +1593,15 @@
       </c>
       <c r="F9" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>12.482758620689655</v>
       </c>
       <c r="G9" s="4">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H9" s="4">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I9" s="4">
         <f t="shared" si="4"/>
@@ -1609,11 +1609,11 @@
       </c>
       <c r="J9" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>12.344827586206897</v>
       </c>
       <c r="K9" s="7">
         <f t="shared" si="6"/>
-        <v>0.20689655172413793</v>
+        <v>3.4482758620689655E-2</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -1633,15 +1633,15 @@
       </c>
       <c r="F10" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>12.344827586206897</v>
       </c>
       <c r="G10" s="4">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H10" s="4">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I10" s="4">
         <f t="shared" si="4"/>
@@ -1649,11 +1649,11 @@
       </c>
       <c r="J10" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>11.344827586206897</v>
       </c>
       <c r="K10" s="7">
         <f t="shared" si="6"/>
-        <v>0.12962962962962962</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -1671,15 +1671,15 @@
       </c>
       <c r="F11" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>11.344827586206897</v>
       </c>
       <c r="G11" s="4">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H11" s="4">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I11" s="4">
         <f t="shared" si="4"/>
@@ -1687,11 +1687,11 @@
       </c>
       <c r="J11" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>10.567049808429118</v>
       </c>
       <c r="K11" s="7">
         <f t="shared" si="6"/>
-        <v>0.12962962962962962</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -1707,15 +1707,15 @@
       <c r="E12" s="3"/>
       <c r="F12" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>10.567049808429118</v>
       </c>
       <c r="G12" s="4">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H12" s="4">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I12" s="4">
         <f t="shared" si="4"/>
@@ -1723,11 +1723,11 @@
       </c>
       <c r="J12" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>10.270753512132822</v>
       </c>
       <c r="K12" s="7">
         <f t="shared" si="6"/>
-        <v>0.12962962962962962</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -1743,15 +1743,15 @@
       <c r="E13" s="3"/>
       <c r="F13" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>10.270753512132822</v>
       </c>
       <c r="G13" s="4">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H13" s="4">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I13" s="4">
         <f t="shared" si="4"/>
@@ -1759,11 +1759,11 @@
       </c>
       <c r="J13" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>9.9744572158365266</v>
       </c>
       <c r="K13" s="7">
         <f t="shared" si="6"/>
-        <v>0.12962962962962962</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -1779,15 +1779,15 @@
       <c r="E14" s="3"/>
       <c r="F14" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>9.9744572158365266</v>
       </c>
       <c r="G14" s="4">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H14" s="4">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I14" s="4">
         <f t="shared" si="4"/>
@@ -1795,11 +1795,11 @@
       </c>
       <c r="J14" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>9.9744572158365266</v>
       </c>
       <c r="K14" s="7">
         <f t="shared" si="6"/>
-        <v>0.12962962962962962</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -1815,15 +1815,15 @@
       <c r="E15" s="3"/>
       <c r="F15" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>9.9744572158365266</v>
       </c>
       <c r="G15" s="4">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H15" s="4">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I15" s="4">
         <f t="shared" si="4"/>
@@ -1831,11 +1831,11 @@
       </c>
       <c r="J15" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>9.9744572158365266</v>
       </c>
       <c r="K15" s="7">
         <f t="shared" si="6"/>
-        <v>0.12962962962962962</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -1851,15 +1851,15 @@
       <c r="E16" s="3"/>
       <c r="F16" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>9.9744572158365266</v>
       </c>
       <c r="G16" s="4">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H16" s="4">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I16" s="4">
         <f t="shared" si="4"/>
@@ -1867,11 +1867,11 @@
       </c>
       <c r="J16" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>9.9744572158365266</v>
       </c>
       <c r="K16" s="7">
         <f t="shared" si="6"/>
-        <v>0.12962962962962962</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -1887,15 +1887,15 @@
       <c r="E17" s="3"/>
       <c r="F17" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>9.9744572158365266</v>
       </c>
       <c r="G17" s="4">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H17" s="4">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I17" s="4">
         <f t="shared" si="4"/>
@@ -1903,11 +1903,11 @@
       </c>
       <c r="J17" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>9.9744572158365266</v>
       </c>
       <c r="K17" s="7">
         <f t="shared" si="6"/>
-        <v>0.12962962962962962</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -1923,15 +1923,15 @@
       <c r="E18" s="3"/>
       <c r="F18" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>9.9744572158365266</v>
       </c>
       <c r="G18" s="4">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H18" s="4">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I18" s="4">
         <f t="shared" si="4"/>
@@ -1939,11 +1939,11 @@
       </c>
       <c r="J18" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>9.9744572158365266</v>
       </c>
       <c r="K18" s="7">
         <f t="shared" si="6"/>
-        <v>0.12962962962962962</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -1959,15 +1959,15 @@
       <c r="E19" s="3"/>
       <c r="F19" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>9.9744572158365266</v>
       </c>
       <c r="G19" s="4">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H19" s="4">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I19" s="4">
         <f t="shared" si="4"/>
@@ -1975,11 +1975,11 @@
       </c>
       <c r="J19" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>9.9744572158365266</v>
       </c>
       <c r="K19" s="7">
         <f t="shared" si="6"/>
-        <v>0.12962962962962962</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -1995,15 +1995,15 @@
       <c r="E20" s="3"/>
       <c r="F20" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>9.9744572158365266</v>
       </c>
       <c r="G20" s="4">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H20" s="4">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I20" s="4">
         <f t="shared" si="4"/>
@@ -2011,11 +2011,11 @@
       </c>
       <c r="J20" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>9.9744572158365266</v>
       </c>
       <c r="K20" s="7">
         <f t="shared" si="6"/>
-        <v>0.12962962962962962</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2031,15 +2031,15 @@
       <c r="E21" s="3"/>
       <c r="F21" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>9.9744572158365266</v>
       </c>
       <c r="G21" s="4">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H21" s="4">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I21" s="4">
         <f t="shared" si="4"/>
@@ -2047,11 +2047,11 @@
       </c>
       <c r="J21" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>9.9744572158365266</v>
       </c>
       <c r="K21" s="7">
         <f t="shared" si="6"/>
-        <v>0.12962962962962962</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2067,15 +2067,15 @@
       <c r="E22" s="3"/>
       <c r="F22" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>9.9744572158365266</v>
       </c>
       <c r="G22" s="4">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H22" s="4">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I22" s="4">
         <f t="shared" si="4"/>
@@ -2083,11 +2083,11 @@
       </c>
       <c r="J22" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>9.9744572158365266</v>
       </c>
       <c r="K22" s="7">
         <f t="shared" si="6"/>
-        <v>0.12962962962962962</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2105,15 +2105,15 @@
       </c>
       <c r="F23" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>9.9744572158365266</v>
       </c>
       <c r="G23" s="4">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H23" s="4">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I23" s="4">
         <f t="shared" si="4"/>
@@ -2121,11 +2121,11 @@
       </c>
       <c r="J23" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>9.4559386973180075</v>
       </c>
       <c r="K23" s="7">
         <f t="shared" si="6"/>
-        <v>0.12962962962962962</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2143,15 +2143,15 @@
       </c>
       <c r="F24" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>9.4559386973180075</v>
       </c>
       <c r="G24" s="4">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H24" s="4">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I24" s="4">
         <f t="shared" si="4"/>
@@ -2159,11 +2159,11 @@
       </c>
       <c r="J24" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>8.6411238825031926</v>
       </c>
       <c r="K24" s="7">
         <f t="shared" si="6"/>
-        <v>0.12962962962962962</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2175,19 +2175,21 @@
         <v>8</v>
       </c>
       <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
+      <c r="D25" s="3">
+        <v>3</v>
+      </c>
       <c r="E25" s="3"/>
       <c r="F25" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8.6411238825031926</v>
       </c>
       <c r="G25" s="4">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H25" s="4">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I25" s="4">
         <f t="shared" si="4"/>
@@ -2195,11 +2197,11 @@
       </c>
       <c r="J25" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>8.3448275862068968</v>
       </c>
       <c r="K25" s="7">
         <f t="shared" si="6"/>
-        <v>0.12962962962962962</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2214,18 +2216,20 @@
         <v>5</v>
       </c>
       <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
+      <c r="E26" s="3">
+        <v>6</v>
+      </c>
       <c r="F26" s="4">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>13.344827586206897</v>
       </c>
       <c r="G26" s="4">
         <f>H25</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H26" s="4">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I26" s="4">
         <f t="shared" si="4"/>
@@ -2233,11 +2237,11 @@
       </c>
       <c r="J26" s="4">
         <f t="shared" si="5"/>
-        <v>3.4444444444444446</v>
+        <v>12.900383141762452</v>
       </c>
       <c r="K26" s="7">
         <f t="shared" si="6"/>
-        <v>0.12962962962962962</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2246,34 +2250,34 @@
         <v>41559</v>
       </c>
       <c r="B27" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="4">
         <f t="shared" si="2"/>
-        <v>3.4444444444444446</v>
+        <v>12.900383141762452</v>
       </c>
       <c r="G27" s="4">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H27" s="4">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I27" s="4">
         <f t="shared" si="4"/>
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="J27" s="4">
         <f t="shared" si="5"/>
-        <v>2.4074074074074074</v>
+        <v>12.641123882503193</v>
       </c>
       <c r="K27" s="7">
         <f t="shared" si="6"/>
-        <v>0.12962962962962962</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2289,27 +2293,27 @@
       <c r="E28" s="3"/>
       <c r="F28" s="4">
         <f t="shared" si="2"/>
-        <v>2.4074074074074074</v>
+        <v>12.641123882503193</v>
       </c>
       <c r="G28" s="4">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H28" s="4">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I28" s="4">
         <f t="shared" si="4"/>
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="J28" s="4">
         <f t="shared" si="5"/>
-        <v>1.3703703703703705</v>
+        <v>12.344827586206897</v>
       </c>
       <c r="K28" s="7">
         <f t="shared" si="6"/>
-        <v>0.12962962962962962</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2325,27 +2329,27 @@
       <c r="E29" s="3"/>
       <c r="F29" s="4">
         <f t="shared" si="2"/>
-        <v>1.3703703703703705</v>
+        <v>12.344827586206897</v>
       </c>
       <c r="G29" s="4">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H29" s="4">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I29" s="4">
         <f t="shared" si="4"/>
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="J29" s="4">
         <f t="shared" si="5"/>
-        <v>0.33333333333333348</v>
+        <v>12.048531289910601</v>
       </c>
       <c r="K29" s="7">
         <f t="shared" si="6"/>
-        <v>0.12962962962962962</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2361,27 +2365,27 @@
       <c r="E30" s="3"/>
       <c r="F30" s="4">
         <f t="shared" si="2"/>
-        <v>0.33333333333333348</v>
+        <v>12.048531289910601</v>
       </c>
       <c r="G30" s="4">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H30" s="4">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I30" s="4">
         <f t="shared" si="4"/>
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="J30" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>11.752234993614305</v>
       </c>
       <c r="K30" s="7">
         <f t="shared" si="6"/>
-        <v>0.12962962962962962</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2397,27 +2401,27 @@
       <c r="E31" s="3"/>
       <c r="F31" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>11.752234993614305</v>
       </c>
       <c r="G31" s="4">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H31" s="4">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I31" s="4">
         <f t="shared" si="4"/>
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="J31" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>11.455938697318009</v>
       </c>
       <c r="K31" s="7">
         <f t="shared" si="6"/>
-        <v>0.12962962962962962</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2433,27 +2437,27 @@
       <c r="E32" s="3"/>
       <c r="F32" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>11.455938697318009</v>
       </c>
       <c r="G32" s="4">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H32" s="4">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I32" s="4">
         <f t="shared" si="4"/>
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="J32" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>11.159642401021713</v>
       </c>
       <c r="K32" s="7">
         <f t="shared" si="6"/>
-        <v>0.12962962962962962</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2469,27 +2473,27 @@
       <c r="E33" s="3"/>
       <c r="F33" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>11.159642401021713</v>
       </c>
       <c r="G33" s="4">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H33" s="4">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I33" s="4">
         <f t="shared" si="4"/>
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="J33" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>10.863346104725418</v>
       </c>
       <c r="K33" s="7">
         <f t="shared" si="6"/>
-        <v>0.12962962962962962</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2505,27 +2509,27 @@
       <c r="E34" s="3"/>
       <c r="F34" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>10.863346104725418</v>
       </c>
       <c r="G34" s="4">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H34" s="4">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I34" s="4">
         <f t="shared" si="4"/>
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="J34" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>10.567049808429122</v>
       </c>
       <c r="K34" s="7">
         <f t="shared" si="6"/>
-        <v>0.12962962962962962</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2541,27 +2545,27 @@
       <c r="E35" s="3"/>
       <c r="F35" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>10.567049808429122</v>
       </c>
       <c r="G35" s="4">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H35" s="4">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I35" s="4">
         <f t="shared" si="4"/>
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="J35" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>10.270753512132826</v>
       </c>
       <c r="K35" s="7">
         <f t="shared" si="6"/>
-        <v>0.12962962962962962</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2577,27 +2581,27 @@
       <c r="E36" s="3"/>
       <c r="F36" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>10.270753512132826</v>
       </c>
       <c r="G36" s="4">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H36" s="4">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I36" s="4">
         <f t="shared" si="4"/>
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="J36" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>9.9744572158365301</v>
       </c>
       <c r="K36" s="7">
         <f t="shared" si="6"/>
-        <v>0.12962962962962962</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2613,27 +2617,27 @@
       <c r="E37" s="3"/>
       <c r="F37" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>9.9744572158365301</v>
       </c>
       <c r="G37" s="4">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H37" s="4">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I37" s="4">
         <f t="shared" si="4"/>
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="J37" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>9.6781609195402343</v>
       </c>
       <c r="K37" s="7">
         <f t="shared" si="6"/>
-        <v>0.12962962962962962</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2649,27 +2653,27 @@
       <c r="E38" s="3"/>
       <c r="F38" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>9.6781609195402343</v>
       </c>
       <c r="G38" s="4">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H38" s="4">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I38" s="4">
         <f t="shared" si="4"/>
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="J38" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>9.3818646232439384</v>
       </c>
       <c r="K38" s="7">
         <f t="shared" si="6"/>
-        <v>0.12962962962962962</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2685,27 +2689,27 @@
       <c r="E39" s="3"/>
       <c r="F39" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>9.3818646232439384</v>
       </c>
       <c r="G39" s="4">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H39" s="4">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I39" s="4">
         <f t="shared" si="4"/>
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="J39" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>9.0855683269476426</v>
       </c>
       <c r="K39" s="7">
         <f t="shared" si="6"/>
-        <v>0.12962962962962962</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2721,27 +2725,27 @@
       <c r="E40" s="3"/>
       <c r="F40" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>9.0855683269476426</v>
       </c>
       <c r="G40" s="4">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H40" s="4">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I40" s="4">
         <f t="shared" si="4"/>
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="J40" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>8.7892720306513468</v>
       </c>
       <c r="K40" s="7">
         <f t="shared" si="6"/>
-        <v>0.12962962962962962</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2757,27 +2761,27 @@
       <c r="E41" s="3"/>
       <c r="F41" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8.7892720306513468</v>
       </c>
       <c r="G41" s="4">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H41" s="4">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I41" s="4">
         <f t="shared" si="4"/>
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="J41" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>8.4929757343550509</v>
       </c>
       <c r="K41" s="7">
         <f t="shared" si="6"/>
-        <v>0.12962962962962962</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2793,27 +2797,27 @@
       <c r="E42" s="3"/>
       <c r="F42" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8.4929757343550509</v>
       </c>
       <c r="G42" s="4">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H42" s="4">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I42" s="4">
         <f t="shared" si="4"/>
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="J42" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>8.1966794380587551</v>
       </c>
       <c r="K42" s="7">
         <f t="shared" si="6"/>
-        <v>0.12962962962962962</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2829,27 +2833,27 @@
       <c r="E43" s="3"/>
       <c r="F43" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8.1966794380587551</v>
       </c>
       <c r="G43" s="4">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H43" s="4">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I43" s="4">
         <f t="shared" si="4"/>
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="J43" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>7.9003831417624593</v>
       </c>
       <c r="K43" s="7">
         <f t="shared" si="6"/>
-        <v>0.12962962962962962</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2865,27 +2869,27 @@
       <c r="E44" s="3"/>
       <c r="F44" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>7.9003831417624593</v>
       </c>
       <c r="G44" s="4">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H44" s="4">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I44" s="4">
         <f t="shared" si="4"/>
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="J44" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>7.6040868454661634</v>
       </c>
       <c r="K44" s="7">
         <f t="shared" si="6"/>
-        <v>0.12962962962962962</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2901,27 +2905,27 @@
       <c r="E45" s="3"/>
       <c r="F45" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>7.6040868454661634</v>
       </c>
       <c r="G45" s="4">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H45" s="4">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I45" s="4">
         <f t="shared" si="4"/>
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="J45" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>7.3077905491698676</v>
       </c>
       <c r="K45" s="7">
         <f t="shared" si="6"/>
-        <v>0.12962962962962962</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2937,27 +2941,27 @@
       <c r="E46" s="3"/>
       <c r="F46" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>7.3077905491698676</v>
       </c>
       <c r="G46" s="4">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H46" s="4">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I46" s="4">
         <f t="shared" si="4"/>
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="J46" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>7.0114942528735718</v>
       </c>
       <c r="K46" s="7">
         <f t="shared" si="6"/>
-        <v>0.12962962962962962</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2973,27 +2977,27 @@
       <c r="E47" s="3"/>
       <c r="F47" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>7.0114942528735718</v>
       </c>
       <c r="G47" s="4">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H47" s="4">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I47" s="4">
         <f t="shared" si="4"/>
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="J47" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>6.7151979565772759</v>
       </c>
       <c r="K47" s="7">
         <f t="shared" si="6"/>
-        <v>0.12962962962962962</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="20.65" customHeight="1" x14ac:dyDescent="0.2">
@@ -3009,43 +3013,43 @@
       <c r="E48" s="3"/>
       <c r="F48" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6.7151979565772759</v>
       </c>
       <c r="G48" s="4">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H48" s="4">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I48" s="4">
         <f t="shared" si="4"/>
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="J48" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>6.4189016602809801</v>
       </c>
       <c r="K48" s="7">
         <f t="shared" si="6"/>
-        <v>0.12962962962962962</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="49" spans="1:11" ht="20.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="8"/>
       <c r="B49" s="9">
         <f>SUM(B3:B27)</f>
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C49" s="9"/>
       <c r="D49" s="9">
         <f>AVERAGE(D3:D48)</f>
-        <v>0.66666666666666663</v>
+        <v>1.25</v>
       </c>
       <c r="E49" s="9">
         <f>AVERAGE(E3:E48)</f>
-        <v>9.0909090909090917</v>
+        <v>8.8333333333333339</v>
       </c>
       <c r="F49" s="9"/>
       <c r="G49" s="9"/>

</xml_diff>

<commit_message>
Planning commit for pull
</commit_message>
<xml_diff>
--- a/01_Planning/ProductBurndown.xlsx
+++ b/01_Planning/ProductBurndown.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1 - Initial" sheetId="1" r:id="rId1"/>
@@ -1119,11 +1119,11 @@
   </sheetPr>
   <dimension ref="A1:IV53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D17" sqref="D17"/>
+      <selection pane="bottomRight" activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2367,7 +2367,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="H8" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H8" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="O37" sqref="O37"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Filter bug and filter tutor comments
</commit_message>
<xml_diff>
--- a/01_Planning/ProductBurndown.xlsx
+++ b/01_Planning/ProductBurndown.xlsx
@@ -476,43 +476,43 @@
                   <c:v>6.4088157152353773</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5.9736692717207331</c:v>
+                  <c:v>6.1912424934780548</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5.9736692717207331</c:v>
+                  <c:v>6.1912424934780548</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5.9736692717207331</c:v>
+                  <c:v>6.1912424934780548</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5.538522828206089</c:v>
+                  <c:v>5.7560960499634106</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5.1033763846914448</c:v>
+                  <c:v>5.3209496064487665</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4.6682299411768007</c:v>
+                  <c:v>4.8858031629341223</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4.2330834976621565</c:v>
+                  <c:v>4.4506567194194782</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>3.7979370541475124</c:v>
+                  <c:v>4.015510275904834</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>3.3627906106328682</c:v>
+                  <c:v>3.5803638323901898</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3.3627906106328682</c:v>
+                  <c:v>3.5803638323901898</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.9276441671182241</c:v>
+                  <c:v>3.1452173888755457</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.4924977236035799</c:v>
+                  <c:v>2.7100709453609015</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.0573512800889358</c:v>
+                  <c:v>2.2749245018462574</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -533,11 +533,11 @@
         </c:dLbls>
         <c:gapWidth val="40"/>
         <c:overlap val="-10"/>
-        <c:axId val="212577112"/>
-        <c:axId val="212576328"/>
+        <c:axId val="187867904"/>
+        <c:axId val="187864376"/>
       </c:barChart>
       <c:dateAx>
-        <c:axId val="212577112"/>
+        <c:axId val="187867904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -576,14 +576,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="212576328"/>
+        <c:crossAx val="187864376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="212576328"/>
+        <c:axId val="187864376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -629,7 +629,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="212577112"/>
+        <c:crossAx val="187867904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="25"/>
@@ -698,7 +698,7 @@
         <xdr:cNvPr id="2" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -734,7 +734,7 @@
         <xdr:cNvPr id="4" name="CustomShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1123,7 +1123,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D22" sqref="D22"/>
+      <selection pane="bottomRight" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1694,7 +1694,9 @@
         <v>2</v>
       </c>
       <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
+      <c r="E16" s="3">
+        <v>12</v>
+      </c>
       <c r="F16" s="4">
         <f t="shared" si="6"/>
         <v>7.061535380507344</v>
@@ -1725,7 +1727,7 @@
         <v>41625</v>
       </c>
       <c r="B17" s="3">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
@@ -1744,11 +1746,11 @@
       </c>
       <c r="I17" s="4">
         <f t="shared" si="3"/>
-        <v>239</v>
+        <v>251</v>
       </c>
       <c r="J17" s="4">
         <f t="shared" si="4"/>
-        <v>5.9736692717207331</v>
+        <v>6.1912424934780548</v>
       </c>
       <c r="K17" s="7">
         <f t="shared" si="5"/>
@@ -1767,7 +1769,7 @@
       <c r="E18" s="3"/>
       <c r="F18" s="4">
         <f t="shared" si="6"/>
-        <v>5.9736692717207331</v>
+        <v>6.1912424934780548</v>
       </c>
       <c r="G18" s="4">
         <f t="shared" si="2"/>
@@ -1779,11 +1781,11 @@
       </c>
       <c r="I18" s="4">
         <f t="shared" si="3"/>
-        <v>239</v>
+        <v>251</v>
       </c>
       <c r="J18" s="4">
         <f t="shared" si="4"/>
-        <v>5.9736692717207331</v>
+        <v>6.1912424934780548</v>
       </c>
       <c r="K18" s="7">
         <f t="shared" si="5"/>
@@ -1802,7 +1804,7 @@
       <c r="E19" s="3"/>
       <c r="F19" s="4">
         <f t="shared" si="6"/>
-        <v>5.9736692717207331</v>
+        <v>6.1912424934780548</v>
       </c>
       <c r="G19" s="4">
         <f t="shared" si="2"/>
@@ -1814,11 +1816,11 @@
       </c>
       <c r="I19" s="4">
         <f t="shared" si="3"/>
-        <v>239</v>
+        <v>251</v>
       </c>
       <c r="J19" s="4">
         <f t="shared" si="4"/>
-        <v>5.9736692717207331</v>
+        <v>6.1912424934780548</v>
       </c>
       <c r="K19" s="7">
         <f t="shared" si="5"/>
@@ -1837,7 +1839,7 @@
       <c r="E20" s="3"/>
       <c r="F20" s="4">
         <f t="shared" si="6"/>
-        <v>5.9736692717207331</v>
+        <v>6.1912424934780548</v>
       </c>
       <c r="G20" s="4">
         <f t="shared" si="2"/>
@@ -1849,11 +1851,11 @@
       </c>
       <c r="I20" s="4">
         <f t="shared" si="3"/>
-        <v>239</v>
+        <v>251</v>
       </c>
       <c r="J20" s="4">
         <f t="shared" si="4"/>
-        <v>5.538522828206089</v>
+        <v>5.7560960499634106</v>
       </c>
       <c r="K20" s="7">
         <f t="shared" si="5"/>
@@ -1872,7 +1874,7 @@
       <c r="E21" s="3"/>
       <c r="F21" s="4">
         <f t="shared" si="6"/>
-        <v>5.538522828206089</v>
+        <v>5.7560960499634106</v>
       </c>
       <c r="G21" s="4">
         <f t="shared" si="2"/>
@@ -1884,11 +1886,11 @@
       </c>
       <c r="I21" s="4">
         <f t="shared" si="3"/>
-        <v>239</v>
+        <v>251</v>
       </c>
       <c r="J21" s="4">
         <f t="shared" si="4"/>
-        <v>5.1033763846914448</v>
+        <v>5.3209496064487665</v>
       </c>
       <c r="K21" s="7">
         <f t="shared" si="5"/>
@@ -1907,7 +1909,7 @@
       <c r="E22" s="3"/>
       <c r="F22" s="4">
         <f t="shared" si="6"/>
-        <v>5.1033763846914448</v>
+        <v>5.3209496064487665</v>
       </c>
       <c r="G22" s="4">
         <f t="shared" si="2"/>
@@ -1919,11 +1921,11 @@
       </c>
       <c r="I22" s="4">
         <f t="shared" si="3"/>
-        <v>239</v>
+        <v>251</v>
       </c>
       <c r="J22" s="4">
         <f t="shared" si="4"/>
-        <v>4.6682299411768007</v>
+        <v>4.8858031629341223</v>
       </c>
       <c r="K22" s="7">
         <f t="shared" si="5"/>
@@ -1942,7 +1944,7 @@
       <c r="E23" s="3"/>
       <c r="F23" s="4">
         <f t="shared" si="6"/>
-        <v>4.6682299411768007</v>
+        <v>4.8858031629341223</v>
       </c>
       <c r="G23" s="4">
         <f t="shared" si="2"/>
@@ -1954,11 +1956,11 @@
       </c>
       <c r="I23" s="4">
         <f t="shared" si="3"/>
-        <v>239</v>
+        <v>251</v>
       </c>
       <c r="J23" s="4">
         <f t="shared" si="4"/>
-        <v>4.2330834976621565</v>
+        <v>4.4506567194194782</v>
       </c>
       <c r="K23" s="7">
         <f t="shared" si="5"/>
@@ -1977,7 +1979,7 @@
       <c r="E24" s="3"/>
       <c r="F24" s="4">
         <f t="shared" si="6"/>
-        <v>4.2330834976621565</v>
+        <v>4.4506567194194782</v>
       </c>
       <c r="G24" s="4">
         <f t="shared" si="2"/>
@@ -1989,11 +1991,11 @@
       </c>
       <c r="I24" s="4">
         <f t="shared" si="3"/>
-        <v>239</v>
+        <v>251</v>
       </c>
       <c r="J24" s="4">
         <f t="shared" si="4"/>
-        <v>3.7979370541475124</v>
+        <v>4.015510275904834</v>
       </c>
       <c r="K24" s="7">
         <f t="shared" si="5"/>
@@ -2012,7 +2014,7 @@
       <c r="E25" s="3"/>
       <c r="F25" s="4">
         <f t="shared" si="6"/>
-        <v>3.7979370541475124</v>
+        <v>4.015510275904834</v>
       </c>
       <c r="G25" s="4">
         <f t="shared" si="2"/>
@@ -2024,11 +2026,11 @@
       </c>
       <c r="I25" s="4">
         <f t="shared" si="3"/>
-        <v>239</v>
+        <v>251</v>
       </c>
       <c r="J25" s="4">
         <f t="shared" si="4"/>
-        <v>3.3627906106328682</v>
+        <v>3.5803638323901898</v>
       </c>
       <c r="K25" s="7">
         <f t="shared" si="5"/>
@@ -2047,7 +2049,7 @@
       <c r="E26" s="3"/>
       <c r="F26" s="4">
         <f t="shared" si="6"/>
-        <v>3.3627906106328682</v>
+        <v>3.5803638323901898</v>
       </c>
       <c r="G26" s="4">
         <f t="shared" si="2"/>
@@ -2059,11 +2061,11 @@
       </c>
       <c r="I26" s="4">
         <f t="shared" si="3"/>
-        <v>239</v>
+        <v>251</v>
       </c>
       <c r="J26" s="4">
         <f t="shared" si="4"/>
-        <v>3.3627906106328682</v>
+        <v>3.5803638323901898</v>
       </c>
       <c r="K26" s="7">
         <f t="shared" si="5"/>
@@ -2082,7 +2084,7 @@
       <c r="E27" s="3"/>
       <c r="F27" s="4">
         <f t="shared" si="6"/>
-        <v>3.3627906106328682</v>
+        <v>3.5803638323901898</v>
       </c>
       <c r="G27" s="4">
         <f t="shared" si="2"/>
@@ -2094,11 +2096,11 @@
       </c>
       <c r="I27" s="4">
         <f t="shared" si="3"/>
-        <v>239</v>
+        <v>251</v>
       </c>
       <c r="J27" s="4">
         <f t="shared" si="4"/>
-        <v>2.9276441671182241</v>
+        <v>3.1452173888755457</v>
       </c>
       <c r="K27" s="7">
         <f t="shared" si="5"/>
@@ -2117,7 +2119,7 @@
       <c r="E28" s="3"/>
       <c r="F28" s="4">
         <f t="shared" si="6"/>
-        <v>2.9276441671182241</v>
+        <v>3.1452173888755457</v>
       </c>
       <c r="G28" s="4">
         <f t="shared" si="2"/>
@@ -2129,11 +2131,11 @@
       </c>
       <c r="I28" s="4">
         <f t="shared" si="3"/>
-        <v>239</v>
+        <v>251</v>
       </c>
       <c r="J28" s="4">
         <f t="shared" si="4"/>
-        <v>2.4924977236035799</v>
+        <v>2.7100709453609015</v>
       </c>
       <c r="K28" s="7">
         <f t="shared" si="5"/>
@@ -2152,7 +2154,7 @@
       <c r="E29" s="3"/>
       <c r="F29" s="4">
         <f t="shared" si="6"/>
-        <v>2.4924977236035799</v>
+        <v>2.7100709453609015</v>
       </c>
       <c r="G29" s="4">
         <f t="shared" si="2"/>
@@ -2164,11 +2166,11 @@
       </c>
       <c r="I29" s="4">
         <f t="shared" si="3"/>
-        <v>239</v>
+        <v>251</v>
       </c>
       <c r="J29" s="4">
         <f t="shared" si="4"/>
-        <v>2.0573512800889358</v>
+        <v>2.2749245018462574</v>
       </c>
       <c r="K29" s="7">
         <f t="shared" si="5"/>
@@ -2187,7 +2189,7 @@
       <c r="E30" s="3"/>
       <c r="F30" s="4">
         <f t="shared" si="6"/>
-        <v>2.0573512800889358</v>
+        <v>2.2749245018462574</v>
       </c>
       <c r="G30" s="4">
         <f t="shared" si="2"/>
@@ -2199,11 +2201,11 @@
       </c>
       <c r="I30" s="4">
         <f t="shared" si="3"/>
-        <v>239</v>
+        <v>251</v>
       </c>
       <c r="J30" s="4">
         <f t="shared" si="4"/>
-        <v>1.6222048365742914</v>
+        <v>1.839778058331613</v>
       </c>
       <c r="K30" s="7">
         <f t="shared" si="5"/>
@@ -2222,7 +2224,7 @@
       <c r="E31" s="3"/>
       <c r="F31" s="4">
         <f t="shared" si="6"/>
-        <v>1.6222048365742914</v>
+        <v>1.839778058331613</v>
       </c>
       <c r="G31" s="4">
         <f t="shared" si="2"/>
@@ -2234,11 +2236,11 @@
       </c>
       <c r="I31" s="4">
         <f t="shared" si="3"/>
-        <v>239</v>
+        <v>251</v>
       </c>
       <c r="J31" s="4">
         <f t="shared" si="4"/>
-        <v>1.187058393059647</v>
+        <v>1.4046316148169686</v>
       </c>
       <c r="K31" s="7">
         <f t="shared" si="5"/>
@@ -2257,7 +2259,7 @@
       <c r="E32" s="3"/>
       <c r="F32" s="4">
         <f t="shared" si="6"/>
-        <v>1.187058393059647</v>
+        <v>1.4046316148169686</v>
       </c>
       <c r="G32" s="4">
         <f t="shared" si="2"/>
@@ -2269,11 +2271,11 @@
       </c>
       <c r="I32" s="4">
         <f t="shared" si="3"/>
-        <v>239</v>
+        <v>251</v>
       </c>
       <c r="J32" s="4">
         <f t="shared" si="4"/>
-        <v>0.75191194954500262</v>
+        <v>0.96948517130232426</v>
       </c>
       <c r="K32" s="7">
         <f t="shared" si="5"/>
@@ -2292,7 +2294,7 @@
       <c r="E33" s="3"/>
       <c r="F33" s="4">
         <f t="shared" si="6"/>
-        <v>0.75191194954500262</v>
+        <v>0.96948517130232426</v>
       </c>
       <c r="G33" s="4">
         <f t="shared" si="2"/>
@@ -2304,11 +2306,11 @@
       </c>
       <c r="I33" s="4">
         <f t="shared" si="3"/>
-        <v>239</v>
+        <v>251</v>
       </c>
       <c r="J33" s="4">
         <f t="shared" si="4"/>
-        <v>0.31676550603035825</v>
+        <v>0.53433872778767988</v>
       </c>
       <c r="K33" s="7">
         <f t="shared" si="5"/>
@@ -2328,7 +2330,7 @@
       </c>
       <c r="E34" s="9">
         <f>AVERAGE(E3:E29)</f>
-        <v>11.461538461538462</v>
+        <v>11.5</v>
       </c>
       <c r="F34" s="9"/>
       <c r="G34" s="9"/>

</xml_diff>

<commit_message>
reviews and reviews accept/reject
</commit_message>
<xml_diff>
--- a/01_Planning/ProductBurndown.xlsx
+++ b/01_Planning/ProductBurndown.xlsx
@@ -497,19 +497,19 @@
                   <c:v>1.893836635737469</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.413836635737469</c:v>
+                  <c:v>1.173836635737469</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.933836635737469</c:v>
+                  <c:v>1.173836635737469</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.933836635737469</c:v>
+                  <c:v>1.173836635737469</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.45383663573746902</c:v>
+                  <c:v>0.81383663573746901</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0</c:v>
+                  <c:v>0.33383663573746902</c:v>
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>0</c:v>
@@ -533,11 +533,11 @@
         </c:dLbls>
         <c:gapWidth val="40"/>
         <c:overlap val="-10"/>
-        <c:axId val="199854496"/>
-        <c:axId val="199857632"/>
+        <c:axId val="224633488"/>
+        <c:axId val="224630744"/>
       </c:barChart>
       <c:dateAx>
-        <c:axId val="199854496"/>
+        <c:axId val="224633488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -576,14 +576,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="199857632"/>
+        <c:crossAx val="224630744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="199857632"/>
+        <c:axId val="224630744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -629,7 +629,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="199854496"/>
+        <c:crossAx val="224633488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="25"/>
@@ -698,7 +698,7 @@
         <xdr:cNvPr id="2" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -734,7 +734,7 @@
         <xdr:cNvPr id="4" name="CustomShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1117,13 +1117,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IV53"/>
+  <dimension ref="A1:IV54"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J26" sqref="J26"/>
+      <selection pane="bottomRight" activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1215,7 +1215,7 @@
         <v>1</v>
       </c>
       <c r="H3" s="4">
-        <f t="shared" ref="H3:H33" si="0">G3+D3</f>
+        <f t="shared" ref="H3:H34" si="0">G3+D3</f>
         <v>1</v>
       </c>
       <c r="I3" s="4">
@@ -1285,7 +1285,7 @@
         <v>18.857142857142858</v>
       </c>
       <c r="G5" s="4">
-        <f t="shared" ref="G5:G33" si="2">H4</f>
+        <f t="shared" ref="G5:G32" si="2">H4</f>
         <v>1</v>
       </c>
       <c r="H5" s="4">
@@ -1293,15 +1293,15 @@
         <v>1</v>
       </c>
       <c r="I5" s="4">
-        <f t="shared" ref="I5:I33" si="3">I4+E4</f>
+        <f t="shared" ref="I5:I32" si="3">I4+E4</f>
         <v>107</v>
       </c>
       <c r="J5" s="4">
-        <f t="shared" ref="J5:J33" si="4">MAX(IF(OR(ISBLANK(D5),ISBLANK(E5)),F5-K4*B5,F5-D5),0)</f>
+        <f t="shared" ref="J5:J32" si="4">MAX(IF(OR(ISBLANK(D5),ISBLANK(E5)),F5-K4*B5,F5-D5),0)</f>
         <v>18.651535380507344</v>
       </c>
       <c r="K5" s="7">
-        <f t="shared" ref="K5:K33" si="5">IF(OR(ISBLANK(D5),ISBLANK(E5)),K4,H5/(I5+E5))</f>
+        <f t="shared" ref="K5:K32" si="5">IF(OR(ISBLANK(D5),ISBLANK(E5)),K4,H5/(I5+E5))</f>
         <v>9.3457943925233638E-3</v>
       </c>
     </row>
@@ -1507,7 +1507,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="4">
-        <f t="shared" ref="F11:F33" si="6">J10+C11</f>
+        <f t="shared" ref="F11:F32" si="6">J10+C11</f>
         <v>11.901535380507344</v>
       </c>
       <c r="G11" s="4">
@@ -1953,7 +1953,9 @@
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
+      <c r="E23" s="3">
+        <v>12</v>
+      </c>
       <c r="F23" s="4">
         <f t="shared" si="6"/>
         <v>2.6138366357374689</v>
@@ -1984,11 +1986,13 @@
         <v>41674</v>
       </c>
       <c r="B24" s="3">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
+      <c r="E24" s="3">
+        <v>3</v>
+      </c>
       <c r="F24" s="4">
         <f t="shared" si="6"/>
         <v>1.893836635737469</v>
@@ -2003,11 +2007,11 @@
       </c>
       <c r="I24" s="4">
         <f t="shared" si="3"/>
-        <v>300</v>
+        <v>312</v>
       </c>
       <c r="J24" s="4">
         <f t="shared" si="4"/>
-        <v>1.413836635737469</v>
+        <v>1.173836635737469</v>
       </c>
       <c r="K24" s="7">
         <f t="shared" si="5"/>
@@ -2019,14 +2023,16 @@
         <v>41681</v>
       </c>
       <c r="B25" s="3">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
+      <c r="E25" s="3">
+        <v>0</v>
+      </c>
       <c r="F25" s="4">
         <f t="shared" si="6"/>
-        <v>1.413836635737469</v>
+        <v>1.173836635737469</v>
       </c>
       <c r="G25" s="4">
         <f t="shared" si="2"/>
@@ -2038,11 +2044,11 @@
       </c>
       <c r="I25" s="4">
         <f t="shared" si="3"/>
-        <v>300</v>
+        <v>315</v>
       </c>
       <c r="J25" s="4">
         <f t="shared" si="4"/>
-        <v>0.933836635737469</v>
+        <v>1.173836635737469</v>
       </c>
       <c r="K25" s="7">
         <f t="shared" si="5"/>
@@ -2058,10 +2064,12 @@
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
+      <c r="E26" s="3">
+        <v>0</v>
+      </c>
       <c r="F26" s="4">
         <f t="shared" si="6"/>
-        <v>0.933836635737469</v>
+        <v>1.173836635737469</v>
       </c>
       <c r="G26" s="4">
         <f t="shared" si="2"/>
@@ -2073,11 +2081,11 @@
       </c>
       <c r="I26" s="4">
         <f t="shared" si="3"/>
-        <v>300</v>
+        <v>315</v>
       </c>
       <c r="J26" s="4">
         <f t="shared" si="4"/>
-        <v>0.933836635737469</v>
+        <v>1.173836635737469</v>
       </c>
       <c r="K26" s="7">
         <f t="shared" si="5"/>
@@ -2089,14 +2097,14 @@
         <v>41695</v>
       </c>
       <c r="B27" s="3">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="4">
         <f t="shared" si="6"/>
-        <v>0.933836635737469</v>
+        <v>1.173836635737469</v>
       </c>
       <c r="G27" s="4">
         <f t="shared" si="2"/>
@@ -2108,11 +2116,11 @@
       </c>
       <c r="I27" s="4">
         <f t="shared" si="3"/>
-        <v>300</v>
+        <v>315</v>
       </c>
       <c r="J27" s="4">
         <f t="shared" si="4"/>
-        <v>0.45383663573746902</v>
+        <v>0.81383663573746901</v>
       </c>
       <c r="K27" s="7">
         <f t="shared" si="5"/>
@@ -2131,7 +2139,7 @@
       <c r="E28" s="3"/>
       <c r="F28" s="4">
         <f t="shared" si="6"/>
-        <v>0.45383663573746902</v>
+        <v>0.81383663573746901</v>
       </c>
       <c r="G28" s="4">
         <f t="shared" si="2"/>
@@ -2143,11 +2151,11 @@
       </c>
       <c r="I28" s="4">
         <f t="shared" si="3"/>
-        <v>300</v>
+        <v>315</v>
       </c>
       <c r="J28" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0.33383663573746902</v>
       </c>
       <c r="K28" s="7">
         <f t="shared" si="5"/>
@@ -2166,7 +2174,7 @@
       <c r="E29" s="3"/>
       <c r="F29" s="4">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.33383663573746902</v>
       </c>
       <c r="G29" s="4">
         <f t="shared" si="2"/>
@@ -2178,7 +2186,7 @@
       </c>
       <c r="I29" s="4">
         <f t="shared" si="3"/>
-        <v>300</v>
+        <v>315</v>
       </c>
       <c r="J29" s="4">
         <f t="shared" si="4"/>
@@ -2213,7 +2221,7 @@
       </c>
       <c r="I30" s="4">
         <f t="shared" si="3"/>
-        <v>300</v>
+        <v>315</v>
       </c>
       <c r="J30" s="4">
         <f t="shared" si="4"/>
@@ -2229,7 +2237,7 @@
         <v>41723</v>
       </c>
       <c r="B31" s="3">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -2248,7 +2256,7 @@
       </c>
       <c r="I31" s="4">
         <f t="shared" si="3"/>
-        <v>300</v>
+        <v>315</v>
       </c>
       <c r="J31" s="4">
         <f t="shared" si="4"/>
@@ -2264,7 +2272,7 @@
         <v>41730</v>
       </c>
       <c r="B32" s="3">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
@@ -2283,7 +2291,7 @@
       </c>
       <c r="I32" s="4">
         <f t="shared" si="3"/>
-        <v>300</v>
+        <v>315</v>
       </c>
       <c r="J32" s="4">
         <f t="shared" si="4"/>
@@ -2305,11 +2313,11 @@
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="4">
-        <f t="shared" si="6"/>
+        <f>J32+C33</f>
         <v>0</v>
       </c>
       <c r="G33" s="4">
-        <f t="shared" si="2"/>
+        <f>H32</f>
         <v>18</v>
       </c>
       <c r="H33" s="4">
@@ -2317,41 +2325,75 @@
         <v>18</v>
       </c>
       <c r="I33" s="4">
-        <f t="shared" si="3"/>
-        <v>300</v>
+        <f>I32+E32</f>
+        <v>315</v>
       </c>
       <c r="J33" s="4">
-        <f t="shared" si="4"/>
+        <f>MAX(IF(OR(ISBLANK(D33),ISBLANK(E33)),F33-K32*B33,F33-D33),0)</f>
         <v>0</v>
       </c>
       <c r="K33" s="7">
-        <f t="shared" si="5"/>
+        <f>IF(OR(ISBLANK(D33),ISBLANK(E33)),K32,H33/(I33+E33))</f>
         <v>0.06</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="8"/>
-      <c r="B34" s="9">
+      <c r="A34" s="5">
+        <v>41744</v>
+      </c>
+      <c r="B34" s="3">
+        <v>8</v>
+      </c>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="4">
+        <f>J33+C34</f>
+        <v>0</v>
+      </c>
+      <c r="G34" s="4">
+        <f>H33</f>
+        <v>18</v>
+      </c>
+      <c r="H34" s="4">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="I34" s="4">
+        <f>I33+E33</f>
+        <v>315</v>
+      </c>
+      <c r="J34" s="4">
+        <f>MAX(IF(OR(ISBLANK(D34),ISBLANK(E34)),F34-K33*B34,F34-D34),0)</f>
+        <v>0</v>
+      </c>
+      <c r="K34" s="7">
+        <f>IF(OR(ISBLANK(D34),ISBLANK(E34)),K33,H34/(I34+E34))</f>
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="8"/>
+      <c r="B35" s="9">
         <f>SUM(B3:B8)</f>
         <v>78</v>
       </c>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9">
+      <c r="C35" s="9"/>
+      <c r="D35" s="9">
         <f>AVERAGE(D3:D29)</f>
         <v>2.8333333333333335</v>
       </c>
-      <c r="E34" s="9">
+      <c r="E35" s="9">
         <f>AVERAGE(E3:E29)</f>
-        <v>11.666666666666666</v>
-      </c>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="9"/>
-      <c r="I34" s="9"/>
-      <c r="J34" s="9"/>
-      <c r="K34" s="10"/>
-    </row>
-    <row r="35" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2"/>
+        <v>10.227272727272727</v>
+      </c>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="9"/>
+      <c r="J35" s="9"/>
+      <c r="K35" s="10"/>
+    </row>
     <row r="36" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="37" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="38" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2364,12 +2406,13 @@
     <row r="45" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="46" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="47" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="1:11" ht="20.65" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="49" ht="20.65" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="50" ht="20.65" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="51" ht="20.65" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="52" ht="20.65" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="53" ht="20.65" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="54" ht="20.65" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:K1"/>

</xml_diff>